<commit_message>
Versão de teste da tela de login, é necessário correção no campo de e-mail na tela de cadastro.
</commit_message>
<xml_diff>
--- a/Logins.xlsx
+++ b/Logins.xlsx
@@ -2,17 +2,89 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t>Azimba</t>
+  </si>
+  <si>
+    <t>xabalabaluba</t>
+  </si>
+  <si>
+    <t>FCV@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Goloko</t>
+  </si>
+  <si>
+    <t>zoiao69</t>
+  </si>
+  <si>
+    <t>ASS@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Danilo</t>
+  </si>
+  <si>
+    <t>Baiuca1</t>
+  </si>
+  <si>
+    <t>zonasul99</t>
+  </si>
+  <si>
+    <t>MOE@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Moe</t>
+  </si>
+  <si>
+    <t>jobijoba</t>
+  </si>
+  <si>
+    <t>bamboleo</t>
+  </si>
+  <si>
+    <t>GSK@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>user06</t>
+  </si>
+  <si>
+    <t>variant01</t>
+  </si>
+  <si>
+    <t>FBX@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Aline</t>
+  </si>
+  <si>
+    <t>user01</t>
+  </si>
+  <si>
+    <t>FBZ@brotherbund.com</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,38 +414,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
corrigido mensagem do user ao efetuar login, agora aparece o exato login e não a posição, adicionado botão voltar em algumas telas e tela de remoção do user.
</commit_message>
<xml_diff>
--- a/Logins.xlsx
+++ b/Logins.xlsx
@@ -1,106 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Azimba</t>
-  </si>
-  <si>
-    <t>xabalabaluba</t>
-  </si>
-  <si>
-    <t>FCV@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Fabio</t>
-  </si>
-  <si>
-    <t>Goloko</t>
-  </si>
-  <si>
-    <t>zoiao69</t>
-  </si>
-  <si>
-    <t>ASS@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Danilo</t>
-  </si>
-  <si>
-    <t>Baiuca1</t>
-  </si>
-  <si>
-    <t>zonasul99</t>
-  </si>
-  <si>
-    <t>MOE@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Moe</t>
-  </si>
-  <si>
-    <t>jobijoba</t>
-  </si>
-  <si>
-    <t>bamboleo</t>
-  </si>
-  <si>
-    <t>GSK@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>user06</t>
-  </si>
-  <si>
-    <t>variant01</t>
-  </si>
-  <si>
-    <t>FBX@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Aline</t>
-  </si>
-  <si>
-    <t>user01</t>
-  </si>
-  <si>
-    <t>FBZ@brotherbund.com</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -119,13 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,119 +407,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>user01</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>variant01</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>FBZ@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ana</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Azimba</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>xabalabaluba</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FCV@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Goloko</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>zoiao69</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ASS@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Danilo</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Baiuca1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>zonasul99</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MOE@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Moe</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>jobijoba</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>bamboleo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GSK@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>user06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>variant01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>FBX@brotherbund.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Aline</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificado código para orientado a objetos, agora, as telas estão sendo mantidas na mesma janela
</commit_message>
<xml_diff>
--- a/Logins.xlsx
+++ b/Logins.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -568,10 +568,13 @@
           <t>Aline</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>23</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
       </c>
     </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>